<commit_message>
template_v6-02: link columns to data dictionary
</commit_message>
<xml_diff>
--- a/templates/internalUseOnly/accdcDataEntryTemplate.xlsx
+++ b/templates/internalUseOnly/accdcDataEntryTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\02.1 - WORK AREAS\AC CDC Data Load\template\templates\internalUseOnly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0615F9D-40A8-4073-B0B3-50987904177A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1C47E4-034F-47E8-B9EC-72370F1C7B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="2325" windowWidth="18000" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template_v6-02" sheetId="1" r:id="rId1"/>
@@ -35,40 +35,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>james</author>
-  </authors>
-  <commentList>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{BAA0ED08-A7F2-4B58-8A07-3FBD9508F9B3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>james:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-0 or 1</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
   <si>
@@ -324,9 +290,6 @@
     <t>CDCOBSERVER</t>
   </si>
   <si>
-    <t>JLC 2020 04 10</t>
-  </si>
-  <si>
     <t>OBTIME</t>
   </si>
   <si>
@@ -334,6 +297,9 @@
   </si>
   <si>
     <t>OBTIMEgeneral</t>
+  </si>
+  <si>
+    <t>JLC 2023 04 10</t>
   </si>
 </sst>
 </file>
@@ -343,7 +309,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,19 +374,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -460,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -484,9 +437,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -840,107 +790,109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="9.42578125" style="15" customWidth="1"/>
-    <col min="11" max="11" width="10" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10" style="15" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11" style="15" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11" style="15" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17" style="15" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9" style="15" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9" style="15" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="8.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9" style="15" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="5.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="10" style="15" bestFit="1" customWidth="1"/>
-    <col min="56" max="57" width="9.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="11.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="59" max="60" width="7.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="11.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="7.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="11.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="11.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="10.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="11" style="15" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="10.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="10.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="22.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="17.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="30.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="7.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="10.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="7.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="8.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="8.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="9.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="9.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="7.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="7.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="8.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="9.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="12" style="15" bestFit="1" customWidth="1"/>
-    <col min="85" max="86" width="8.85546875" style="15"/>
-    <col min="87" max="87" width="19.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="88" max="141" width="4.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="142" max="147" width="3.7109375" style="15" customWidth="1"/>
-    <col min="148" max="16384" width="8.85546875" style="15"/>
+    <col min="1" max="1" width="6.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.42578125" style="14" customWidth="1"/>
+    <col min="11" max="11" width="10" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10" style="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17" style="14" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9" style="14" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9" style="14" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="8.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="9" style="14" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="5.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="8.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="10" style="14" bestFit="1" customWidth="1"/>
+    <col min="56" max="57" width="9.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="11.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="59" max="60" width="7.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="11.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="7.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="11.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="10.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="10.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="10.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="22.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="17.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="30.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="7.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="10.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="7.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="8.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="8.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="9.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="9.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="7.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="7.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="8.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="9.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="12" style="14" bestFit="1" customWidth="1"/>
+    <col min="85" max="86" width="8.85546875" style="14"/>
+    <col min="87" max="87" width="19.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="88" max="141" width="4.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="142" max="147" width="3.7109375" style="14" customWidth="1"/>
+    <col min="148" max="16384" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:147" s="2" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>75</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -952,7 +904,7 @@
       <c r="F1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>76</v>
       </c>
       <c r="H1" s="8" t="s">
@@ -964,20 +916,20 @@
       <c r="J1" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="16" t="s">
         <v>6</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>77</v>
       </c>
       <c r="M1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>87</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>2</v>
@@ -1003,25 +955,25 @@
       <c r="W1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Y1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AB1" s="10" t="s">
+      <c r="AB1" s="9" t="s">
         <v>59</v>
       </c>
       <c r="AC1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="AD1" s="9" t="s">
         <v>60</v>
       </c>
       <c r="AE1" s="8" t="s">
@@ -1030,16 +982,16 @@
       <c r="AF1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="AG1" s="10" t="s">
+      <c r="AG1" s="9" t="s">
         <v>58</v>
       </c>
       <c r="AH1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="10" t="s">
+      <c r="AI1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="AJ1" s="17" t="s">
+      <c r="AJ1" s="16" t="s">
         <v>31</v>
       </c>
       <c r="AK1" s="8" t="s">
@@ -1114,79 +1066,79 @@
       <c r="BH1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="BI1" s="11" t="s">
+      <c r="BI1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="BJ1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="BK1" s="18" t="s">
+      <c r="BJ1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="BK1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="BL1" s="18" t="s">
+      <c r="BL1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="BM1" s="18" t="s">
+      <c r="BM1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="BN1" s="11" t="s">
+      <c r="BN1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="BO1" s="12" t="s">
+      <c r="BO1" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="BP1" s="12" t="s">
+      <c r="BP1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="BQ1" s="18" t="s">
+      <c r="BQ1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="BR1" s="12" t="s">
+      <c r="BR1" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="BS1" s="12" t="s">
+      <c r="BS1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="BT1" s="11" t="s">
+      <c r="BT1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="BU1" s="11" t="s">
+      <c r="BU1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="BV1" s="11" t="s">
+      <c r="BV1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="BW1" s="11" t="s">
+      <c r="BW1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="BX1" s="11" t="s">
+      <c r="BX1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="BY1" s="11" t="s">
+      <c r="BY1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="BZ1" s="11" t="s">
+      <c r="BZ1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="CA1" s="11" t="s">
+      <c r="CA1" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="CB1" s="11" t="s">
+      <c r="CB1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="CC1" s="11" t="s">
+      <c r="CC1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="CD1" s="11" t="s">
+      <c r="CD1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="CE1" s="11" t="s">
+      <c r="CE1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="CF1" s="11" t="s">
+      <c r="CF1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="CI1" s="13" t="s">
+      <c r="CI1" s="12" t="s">
         <v>65</v>
       </c>
       <c r="CJ1" s="2">
@@ -1510,10 +1462,10 @@
       <c r="BF2" s="1"/>
       <c r="BG2" s="1"/>
       <c r="BH2" s="1"/>
-      <c r="BI2" s="14"/>
+      <c r="BI2" s="13"/>
       <c r="BJ2" s="6" t="str">
         <f>B2&amp;"_"&amp;BF2&amp;"_"&amp;BO2</f>
-        <v>__201011</v>
+        <v>__231011</v>
       </c>
       <c r="BK2" s="6" t="str">
         <f>IF(Z2="","point","line")</f>
@@ -1531,14 +1483,14 @@
         <v>51</v>
       </c>
       <c r="BO2" s="6">
-        <v>201011</v>
+        <v>231011</v>
       </c>
       <c r="BP2" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="BQ2" s="6" t="str">
         <f>"ACCDC    "&amp;BP2&amp;"    QC,GIS"</f>
-        <v>ACCDC    JLC 2020 04 10    QC,GIS</v>
+        <v>ACCDC    JLC 2023 04 10    QC,GIS</v>
       </c>
       <c r="BR2" s="6" t="s">
         <v>81</v>
@@ -1807,8 +1759,64 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" location="REFNUM" xr:uid="{3A789CE3-BCB3-4AB8-8492-B9A132EFAA36}"/>
+    <hyperlink ref="D1" r:id="rId2" location="yyyy" xr:uid="{CF531837-54D7-47C7-991C-C8923F8600AF}"/>
+    <hyperlink ref="E1" r:id="rId3" location="mm" xr:uid="{C7331700-9B37-4945-8B9E-E4386B7889CB}"/>
+    <hyperlink ref="F1" r:id="rId4" location="dd" xr:uid="{144B07A8-20C7-4B8C-A6EC-61F5911F6513}"/>
+    <hyperlink ref="H1" r:id="rId5" location="yyyy2" xr:uid="{1F0A47C0-E09F-4186-9A0C-FF2BB1072D32}"/>
+    <hyperlink ref="I1" r:id="rId6" location="mm2" xr:uid="{AC41FECD-8F24-4843-AC89-284B8A96091A}"/>
+    <hyperlink ref="J1" r:id="rId7" location="dd2" xr:uid="{E27BF887-E6B3-4B25-8B57-A9C75F0F6C8E}"/>
+    <hyperlink ref="K1" r:id="rId8" location="obdate" xr:uid="{BB044414-97E4-44CC-A09D-4019AD6036A6}"/>
+    <hyperlink ref="L1" r:id="rId9" location="obdateverbatim" xr:uid="{A2D6C3CA-1BAF-40D4-A8D0-E569C7C904A1}"/>
+    <hyperlink ref="M1" r:id="rId10" location="obtime" xr:uid="{37E4E64F-0DCD-4D42-B9CC-2D6F3DFFBFE0}"/>
+    <hyperlink ref="N1" r:id="rId11" location="obtimeend" xr:uid="{06FE8D34-977B-4493-A4EC-2E9E557ACE95}"/>
+    <hyperlink ref="P1" r:id="rId12" location="elcode" xr:uid="{4D53CB8B-6F81-4BB5-8E6C-3EFFD0B4E7FF}"/>
+    <hyperlink ref="Q1" r:id="rId13" location="nname-sciname" xr:uid="{E170E7FC-15B4-4272-A8F0-362D59F3D4D1}"/>
+    <hyperlink ref="R1" r:id="rId14" location="nametemp" xr:uid="{6B271864-FFBD-4A5C-B6A4-C26595AB9615}"/>
+    <hyperlink ref="S1" r:id="rId15" location="notetax" xr:uid="{D9748356-90D8-4D59-A0C0-6AD5B31D0329}"/>
+    <hyperlink ref="T1" r:id="rId16" location="other-features" xr:uid="{0C25E75D-BB33-4891-A50B-CE0258DE929C}"/>
+    <hyperlink ref="U1" r:id="rId17" location="observer" xr:uid="{E95E85EB-8D55-4C9C-A514-50823C11B4C5}"/>
+    <hyperlink ref="V1" r:id="rId18" location="cdcobserver" xr:uid="{F1A93670-39D4-40EE-9D65-793938A2AF4E}"/>
+    <hyperlink ref="W1" r:id="rId19" location="IDENTBY" xr:uid="{248776F7-81E5-499B-BFA2-80751D0F4B48}"/>
+    <hyperlink ref="X1" r:id="rId20" location="latdec" xr:uid="{65BD6E36-341E-416C-8D2C-EE33DA341616}"/>
+    <hyperlink ref="Y1" r:id="rId21" location="londec" xr:uid="{B2E87300-9C66-4648-9AA9-F3124BB0C333}"/>
+    <hyperlink ref="Z1" r:id="rId22" location="latdec2" xr:uid="{9D355435-3730-47A4-81FC-660F7EE49E18}"/>
+    <hyperlink ref="AA1" r:id="rId23" location="londec2" xr:uid="{B2513D8E-E0DD-47A1-8D42-88F2C336933B}"/>
+    <hyperlink ref="AB1" r:id="rId24" location="_noteloccoordinates" xr:uid="{47677867-EE9E-4138-A56A-B48687851131}"/>
+    <hyperlink ref="AC1" r:id="rId25" location="locuncm" xr:uid="{2DAFF86D-4943-45E8-8682-4668CE86CED3}"/>
+    <hyperlink ref="AD1" r:id="rId26" location="_noteloclocuncm" xr:uid="{FF7400D6-7240-4258-8840-4D3092B86581}"/>
+    <hyperlink ref="AE1" r:id="rId27" location="subnat" xr:uid="{C416D4C4-286B-466F-B15E-D0D8C28DE6F1}"/>
+    <hyperlink ref="AF1" r:id="rId28" location="surveysite" xr:uid="{DA173407-C1D8-4557-869A-C05D2D90B29E}"/>
+    <hyperlink ref="AG1" r:id="rId29" location="_notelocsurveysite" xr:uid="{1705E9BC-DE76-4298-8DB8-CD003FB73F93}"/>
+    <hyperlink ref="AH1" r:id="rId30" location="directions" xr:uid="{01A35A6C-B5BD-4BB0-BEC2-C2EEB267E0B8}"/>
+    <hyperlink ref="AI1" r:id="rId31" location="_notelocdirections" xr:uid="{2FA21417-15BF-4CEC-A3E6-92E41F2D22CC}"/>
+    <hyperlink ref="AK1" r:id="rId32" location="sitecode" xr:uid="{B3CB66AF-9070-41C7-9FA0-F82901505446}"/>
+    <hyperlink ref="AL1" r:id="rId33" location="elevmin" xr:uid="{937393A3-C496-48EF-A536-F603AC41E73F}"/>
+    <hyperlink ref="AM1" r:id="rId34" location="obevid" xr:uid="{23554404-C0FB-4254-8CF0-8A0F7A97338E}"/>
+    <hyperlink ref="AN1" r:id="rId35" location="obabun" xr:uid="{AF049E18-3EB1-4BF1-B97C-CE2184001C9E}"/>
+    <hyperlink ref="AO1" r:id="rId36" location="obabunsite" xr:uid="{78FE3A62-AB6C-4306-8092-34F4D0F305D2}"/>
+    <hyperlink ref="AP1" r:id="rId37" location="obcount" xr:uid="{698B3890-47C1-471C-A09B-D55298FB4A69}"/>
+    <hyperlink ref="AQ1" r:id="rId38" location="obassp" xr:uid="{0AD1F5C5-3D94-48E7-9124-26C5983FE8AB}"/>
+    <hyperlink ref="AR1" r:id="rId39" location="obdesc" xr:uid="{1072177C-A769-496E-91E2-03F9EE41C821}"/>
+    <hyperlink ref="AS1" r:id="rId40" location="obactiv" xr:uid="{F594096C-5BCA-43E4-8889-76EAF4F04AA2}"/>
+    <hyperlink ref="AT1" r:id="rId41" location="obphen" xr:uid="{5F0C2F3C-727E-4D31-A34D-09E96A65581A}"/>
+    <hyperlink ref="AU1" r:id="rId42" location="obsex" xr:uid="{541BF94E-43F2-48DD-AA31-D2FFD3934D38}"/>
+    <hyperlink ref="AV1" r:id="rId43" location="habitat" xr:uid="{F7700491-7896-4E4A-92F2-748706BA776B}"/>
+    <hyperlink ref="AW1" r:id="rId44" location="obthreat" xr:uid="{82A69B00-4992-4F14-8F4F-80D81932D714}"/>
+    <hyperlink ref="AX1" r:id="rId45" location="environmental" xr:uid="{BE2349AD-A46C-4C62-8499-AA96CDA4518A}"/>
+    <hyperlink ref="AY1" r:id="rId46" location="url" xr:uid="{67164F57-E25E-40CA-B951-57F015CE9ADB}"/>
+    <hyperlink ref="AZ1" r:id="rId47" location="project" xr:uid="{53A5845E-9D31-4F75-89FC-2679811D520F}"/>
+    <hyperlink ref="BA1" r:id="rId48" location="protocol" xr:uid="{9CF199A5-FCA5-440F-B3FD-BA9EA43B1576}"/>
+    <hyperlink ref="BB1" r:id="rId49" location="collection" xr:uid="{BF61C842-7AFD-40A9-8D77-496BCD6554B2}"/>
+    <hyperlink ref="BC1" r:id="rId50" location="collnum" xr:uid="{8C419C1E-1160-4787-8828-B2E5F3B7F89F}"/>
+    <hyperlink ref="BD1" r:id="rId51" location="colldup" xr:uid="{2DA43184-77D7-4F5F-B1ED-78707ACD35E6}"/>
+    <hyperlink ref="BE1" r:id="rId52" location="accnum" xr:uid="{0C9B3CAB-E57F-4DC8-847D-90791BFB663E}"/>
+    <hyperlink ref="BF1" r:id="rId53" location="bestsource" xr:uid="{8648C3E6-7B70-4E28-B028-4447C374D9B2}"/>
+    <hyperlink ref="BG1" r:id="rId54" location="note1" xr:uid="{72DD2237-11D7-4510-BF02-A5803DD53BF4}"/>
+    <hyperlink ref="BH1" r:id="rId55" location="note2" xr:uid="{3AD7BEC1-22A2-465B-A36C-45E263833206}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId56"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change default MAINHIST to CKR
</commit_message>
<xml_diff>
--- a/templates/internalUseOnly/accdcDataEntryTemplate.xlsx
+++ b/templates/internalUseOnly/accdcDataEntryTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\02.1 - WORK AREAS\AC CDC Data Load\template\templates\internalUseOnly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\02.1 - WORK AREAS\copiedToHarddrive\AC CDC Data Load\template\templates\internalUseOnly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BD7D10-C064-4489-8ACA-C1FC50F4251B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D5255F-4408-4422-B6D8-78DADCEAE4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2550" yWindow="240" windowWidth="26010" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template_v6-03" sheetId="1" r:id="rId1"/>
@@ -287,9 +287,6 @@
     <t>OBTIMEgeneral</t>
   </si>
   <si>
-    <t>JLC 2023 04 10</t>
-  </si>
-  <si>
     <t>NOTELOCcoordinates</t>
   </si>
   <si>
@@ -300,6 +297,9 @@
   </si>
   <si>
     <t>NOTELOCdirections</t>
+  </si>
+  <si>
+    <t>CKR 2023 04 10</t>
   </si>
 </sst>
 </file>
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AI1" sqref="AI1"/>
+    <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
+      <selection activeCell="BP2" sqref="BP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -861,7 +861,7 @@
     <col min="65" max="65" width="10.28515625" style="14" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="11" style="14" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="10.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="10.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="14.28515625" style="14" customWidth="1"/>
     <col min="69" max="69" width="22.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="17.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="30.140625" style="14" bestFit="1" customWidth="1"/>
@@ -968,13 +968,13 @@
         <v>56</v>
       </c>
       <c r="AB1" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AC1" s="8" t="s">
         <v>54</v>
       </c>
       <c r="AD1" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AE1" s="8" t="s">
         <v>62</v>
@@ -983,13 +983,13 @@
         <v>16</v>
       </c>
       <c r="AG1" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AH1" s="8" t="s">
         <v>17</v>
       </c>
       <c r="AI1" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AJ1" s="16" t="s">
         <v>31</v>
@@ -1478,11 +1478,11 @@
         <v>231011</v>
       </c>
       <c r="BP2" s="6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="BQ2" s="6" t="str">
         <f>"ACCDC    "&amp;BP2&amp;"    QC,GIS"</f>
-        <v>ACCDC    JLC 2023 04 10    QC,GIS</v>
+        <v>ACCDC    CKR 2023 04 10    QC,GIS</v>
       </c>
       <c r="BR2" s="6" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
update EDITION initials (sorry Charity)
</commit_message>
<xml_diff>
--- a/templates/internalUseOnly/accdcDataEntryTemplate.xlsx
+++ b/templates/internalUseOnly/accdcDataEntryTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pende\Documents\02.1 - WORK AREAS\copiedToHarddrive\AC CDC Data Load\template\templates\internalUseOnly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\arcgisProcessing\dataIn\template_repo\template\templates\internalUseOnly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D5255F-4408-4422-B6D8-78DADCEAE4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943E42F5-CC1F-433E-918E-EFF91EFDA7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="240" windowWidth="26010" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template_v6-03" sheetId="1" r:id="rId1"/>
@@ -299,7 +299,7 @@
     <t>NOTELOCdirections</t>
   </si>
   <si>
-    <t>CKR 2023 04 10</t>
+    <t>JLC 2023 04 10</t>
   </si>
 </sst>
 </file>
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
-      <selection activeCell="BP2" sqref="BP2"/>
+    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
+      <selection activeCell="BP4" sqref="BP4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="BQ2" s="6" t="str">
         <f>"ACCDC    "&amp;BP2&amp;"    QC,GIS"</f>
-        <v>ACCDC    CKR 2023 04 10    QC,GIS</v>
+        <v>ACCDC    JLC 2023 04 10    QC,GIS</v>
       </c>
       <c r="BR2" s="6" t="s">
         <v>77</v>

</xml_diff>